<commit_message>
updated excel_importer to be a class that extends dbservice. Changed import_df_to_db function to use excel_reader function, create a connection, add to db, then close connection. Changed main.py to replace read with import that includes read.
</commit_message>
<xml_diff>
--- a/InheritanceProject/data/excel_input/BeverageList1.xlsx
+++ b/InheritanceProject/data/excel_input/BeverageList1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -40,7 +40,10 @@
     <t xml:space="preserve">ibu</t>
   </si>
   <si>
-    <t xml:space="preserve">grape_varietalcountry</t>
+    <t xml:space="preserve">grape_varietal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">country</t>
   </si>
   <si>
     <t xml:space="preserve">volume_ml</t>
@@ -112,6 +115,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -182,12 +186,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -316,219 +320,222 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="n">
+    </row>
+    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>11.2</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="2" t="n">
         <v>11.99</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="n">
+    </row>
+    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="n">
         <v>25.36</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="2" t="n">
         <v>44.99</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="2" t="n">
         <v>13.5</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="1" t="n">
+      <c r="H3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="2" t="n">
         <v>750</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+    <row r="4" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>18.99</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>25.36</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>10.99</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>14.2</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>9.99</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>11.99</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>10.99</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>25.36</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>9.99</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>18.99</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>1.79</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>25.36</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>10.99</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>14.2</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>9.99</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="C8" s="2" t="n">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>11.99</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="1" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>10.99</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="1" t="n">
-        <v>25.36</v>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>9.99</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" s="1" t="n">
+      <c r="I11" s="2" t="n">
         <v>750</v>
       </c>
     </row>

</xml_diff>